<commit_message>
correct the regex in menu_writer
</commit_message>
<xml_diff>
--- a/new_merged_menu.xlsx
+++ b/new_merged_menu.xlsx
@@ -25,184 +25,190 @@
     <t>Vegetarisch</t>
   </si>
   <si>
-    <t>12.06.2023</t>
-  </si>
-  <si>
-    <t>13.06.2023</t>
-  </si>
-  <si>
-    <t>14.06.2023</t>
-  </si>
-  <si>
-    <t>15.06.2023</t>
-  </si>
-  <si>
-    <t>16.06.2023</t>
-  </si>
-  <si>
-    <t>05.06.2023</t>
-  </si>
-  <si>
-    <t>06.06.2023</t>
-  </si>
-  <si>
-    <t>07.06.2023</t>
-  </si>
-  <si>
-    <t>08.06.2023</t>
-  </si>
-  <si>
-    <t>09.06.2023</t>
-  </si>
-  <si>
-    <t>19.06.2023</t>
-  </si>
-  <si>
-    <t>20.06.2023</t>
-  </si>
-  <si>
-    <t>21.06.2023</t>
-  </si>
-  <si>
-    <t>22.06.2023</t>
-  </si>
-  <si>
-    <t>23.06.2023</t>
-  </si>
-  <si>
-    <t>26.06.2023</t>
-  </si>
-  <si>
-    <t>27.06.2023</t>
-  </si>
-  <si>
-    <t>28.06.2023</t>
-  </si>
-  <si>
-    <t>29.06.2023</t>
-  </si>
-  <si>
-    <t>30.06.2023</t>
-  </si>
-  <si>
-    <t>Penne a,a-1,2 ger. Putenbrust 1,2,16 Gemüse-Sahnesoße g,pFroop g,p</t>
-  </si>
-  <si>
-    <t>Putengyros 2 Tzatziki g,pReis Tomaten-Gurkensalat Apfel 14</t>
-  </si>
-  <si>
-    <t>Gemüse-Quiche mit Räu-chelachs a,c,d,g,p,a-1Salatbeilage c,g,k,pZitronenkuchen a,c,a-1,2</t>
-  </si>
-  <si>
-    <t>Chicken Nuggets a,a-1,16 Ananassauce 8 Gemüsereis Pfirsich</t>
-  </si>
-  <si>
-    <t>Mini Ofenkartoffeln 2 Räucherlachs-Meerrettich-Quark d,g,m,p,2,13 Salatbeilage c,g,k,pSchokopudding g,p</t>
-  </si>
-  <si>
-    <t>Nudel-Gemüseauflauf m. Fleisch a,g,p,a-1,2 Tomaten-Kräuterpestosoße 2 Joghurt m. Kirsche g,p,2</t>
-  </si>
-  <si>
-    <t>Asia-Geschnetzeltes vom Huhn i,m,2,6,13 Reis Banane</t>
-  </si>
-  <si>
-    <t>Hackfleischmasse - Frikadel-le/Hackbraten (Rind) a,c,k,a-1Joghurt-Minz-Dip g,pGemüse Couscous a,i,a-1Apfelkuchen a,c,a-1,2,14</t>
-  </si>
-  <si>
-    <t>Hähnchenbrust paniert a,a-1Bratensoße Kartoffelpüree g,m,p,2 Sommergemüse Birne 14</t>
-  </si>
-  <si>
-    <t>Fischfilet Piccata a,c,d,g,p,a-1Farfalle (Pasta/Nudeln) a,a-1,2 Tomatisierte Zucchini Pudding Sahne c,g,p</t>
-  </si>
-  <si>
-    <t>Gemüseeintopf m. Kartoffel iRauchfleisch (50g) 1,2 Baguette a,a-1Quarkspeise m. Pfirsich g,p</t>
-  </si>
-  <si>
-    <t>Gnocchi-Gemüse-Pfanne c,2 Käsesoße g,p,12 Hähnchenbruststreifen (80g) Birne 14</t>
-  </si>
-  <si>
-    <t>Kichererbsen-Gemüseragout iRindfleisch Couscous a,i,a-1Streuselkuchen a,c,g,p,a-1,2</t>
-  </si>
-  <si>
-    <t>Lasagne Bolognese a,c,g,i,p,a-1,2 Fruchtige Tomatensoße a,a-5Bohnensalat Banane</t>
-  </si>
-  <si>
-    <t>Matjesfilettopf "Hausfrauen Art" c,d,g,k,p,1,3,4,12 Röstkartoffeln 2 Salatbeilage c,g,k,pGötterspeise 12</t>
-  </si>
-  <si>
-    <t>Chili con Carne (Rind) 1 Baguette a,a-1Frucht - Joghurt Dessert g,p</t>
-  </si>
-  <si>
-    <t>Lyoner Wurstsalat i,k,1,2,4,16 Röstkartoffeln 2 Apfel 14</t>
-  </si>
-  <si>
-    <t>Putenkeule geschmort a,c,f,g,i,k,p,2 Champignon-Gemüsesoße g,pSpätzle a,c,a-1Pfirsichkuchen a,c,a-1,2</t>
-  </si>
-  <si>
-    <t>Bauernfrühstück c,g,p,1,2,16 Gewürzgurke 1,4 Salatbeilage c,g,k,pHonigmelone</t>
-  </si>
-  <si>
-    <t>Fischstäbchen a,d,a-1Mayonaise-Kartoffelsalat c,k,12 Vanillepudding g,p,12</t>
-  </si>
-  <si>
-    <t>Penne a,a-1,2 geriebener Käse g,pGemüse-Sahnesoße g,pFroop g,p</t>
-  </si>
-  <si>
-    <t>gebackener Hirtenkäse g,pTzatziki g,pReis Tomaten-Gurkensalat Apfel 14</t>
-  </si>
-  <si>
-    <t>Gemüse-Quiche a,c,g,p,a-1Kräuter-Dip g,pSalatbeilage c,g,k,pZitronenkuchen a,c,a-1,2</t>
-  </si>
-  <si>
-    <t>gebackene Frühlingsrolle a,c,f,a-1Ananassauce 8 Gemüsereis Pfirsich</t>
-  </si>
-  <si>
-    <t>Käsespätzle a,c,g,p,a-1Geschmolzene Zwiebeln 2 Salatbeilage c,g,k,pSchokopudding g,p</t>
-  </si>
-  <si>
-    <t>Nudel-Gemüseauflauf a,g,p,a-1,2 Tomaten-Kräuterpestosoße 2 Joghurt m. Kirsche g,p,2</t>
-  </si>
-  <si>
-    <t>Asia-Geschnetzeltes mit To-fu f,i,m,2,6,13 Reis Banane</t>
-  </si>
-  <si>
-    <t>Falafelbällchen a,a-1Joghurt-Minz-Dip g,pGemüse Couscous a,i,a-1Apfelkuchen a,c,a-1,2,14</t>
-  </si>
-  <si>
-    <t>Milchreis g,pheiße Kirschen Birne 14</t>
-  </si>
-  <si>
-    <t>Zucchini Piccata a,c,g,p,a-1Tomaten-Basilikumsauce g,p,2 Farfalle (Pasta/Nudeln) a,a-1,2 Pudding Sahne c,g,p</t>
-  </si>
-  <si>
-    <t>Gemüseeintopf m. Kartoffel iBaguette a,a-1Quarkspeise m. Pfirsich g,p</t>
-  </si>
-  <si>
-    <t>Gnocchi-Gemüse-Pfanne c,2 Käsesoße g,p,12 Birne 14</t>
-  </si>
-  <si>
-    <t>Kichererbsen-Gemüseragout iCouscous a,i,a-1Streuselkuchen a,c,g,p,a-1,2</t>
-  </si>
-  <si>
-    <t>Gemüselasagne a,c,g,p,a-1,2 Fruchtige Tomatensoße a,a-5Bohnensalat Banane</t>
-  </si>
-  <si>
-    <t>Dampfnudel a,c,g,p,a-1Vanillesoße g,p,12 Götterspeise 12</t>
-  </si>
-  <si>
-    <t>Chili sin Carne (Vegetarisch) a,f,a-1,a-5,1 Baguette a,a-1Frucht - Joghurt Dessert g,p</t>
-  </si>
-  <si>
-    <t>Gemüsefrikadelle a,b,c,e,f,g,h,i,k,l,m,p,a-1Schnittlauchquark g,pRöstkartoffeln 2 Apfel 14</t>
-  </si>
-  <si>
-    <t>Spätzle a,c,a-1Champignon-Gemüseragout g,pPfirsichkuchen a,c,a-1,2</t>
-  </si>
-  <si>
-    <t>Bauernfrühstück VEG c,g,pGewürzgurke 1,4 Salatbeilage c,g,k,pHonigmelone</t>
-  </si>
-  <si>
-    <t>Gemüsestäbchen gebraten a,c,g,i,p,a-1Mayonaise-Kartoffelsalat c,k,12 Vanillepudding g,p,12</t>
+    <t>2023-06-05</t>
+  </si>
+  <si>
+    <t>2023-06-06</t>
+  </si>
+  <si>
+    <t>2023-06-07</t>
+  </si>
+  <si>
+    <t>2023-06-08</t>
+  </si>
+  <si>
+    <t>2023-06-09</t>
+  </si>
+  <si>
+    <t>2023-06-12</t>
+  </si>
+  <si>
+    <t>2023-06-13</t>
+  </si>
+  <si>
+    <t>2023-06-14</t>
+  </si>
+  <si>
+    <t>2023-06-15</t>
+  </si>
+  <si>
+    <t>2023-06-16</t>
+  </si>
+  <si>
+    <t>2023-06-19</t>
+  </si>
+  <si>
+    <t>2023-06-20</t>
+  </si>
+  <si>
+    <t>2023-06-21</t>
+  </si>
+  <si>
+    <t>2023-06-22</t>
+  </si>
+  <si>
+    <t>2023-06-23</t>
+  </si>
+  <si>
+    <t>2023-06-26</t>
+  </si>
+  <si>
+    <t>2023-06-27</t>
+  </si>
+  <si>
+    <t>2023-06-28</t>
+  </si>
+  <si>
+    <t>2023-06-29</t>
+  </si>
+  <si>
+    <t>2023-06-30</t>
+  </si>
+  <si>
+    <t>Nudel-Gemüseauflauf m. Fleisch a,g,p,a-1,2  Tomaten-Kräuterpestosoße 2  Joghurt m. Kirsche g,p,2</t>
+  </si>
+  <si>
+    <t>Asia-Geschnetzeltes vom Huhn i,m,2,6,13  Reis  Banane</t>
+  </si>
+  <si>
+    <t>Hackfleischmasse - Frikadel-
+le/Hackbraten (Rind) a,c,k,a-1 Joghurt-Minz-Dip g,p Gemüse Couscous a,i,a-1 Apfelkuchen a,c,a-1,2,14</t>
+  </si>
+  <si>
+    <t>Hähnchenbrust paniert a,a-1 Bratensoße  Kartoffelpüree g,m,p,2  Sommergemüse  Birne 14</t>
+  </si>
+  <si>
+    <t>Fischfilet Piccata a,c,d,g,p,a-1 Farfalle (Pasta/Nudeln) a,a-1,2  Tomatisierte Zucchini  Pudding Sahne c,g,p</t>
+  </si>
+  <si>
+    <t>Penne a,a-1,2  ger. Putenbrust 1,2,16  Gemüse-Sahnesoße g,p Froop g,p</t>
+  </si>
+  <si>
+    <t>Putengyros 2  Tzatziki g,p Reis  Tomaten-Gurkensalat  Apfel 14</t>
+  </si>
+  <si>
+    <t>Gemüse-Quiche mit Räu-
+chelachs a,c,d,g,p,a-1 Salatbeilage c,g,k,p Zitronenkuchen a,c,a-1,2</t>
+  </si>
+  <si>
+    <t>Chicken Nuggets a,a-1,16  Ananassauce 8  Gemüsereis  Pfirsich</t>
+  </si>
+  <si>
+    <t>Mini Ofenkartoffeln 2  Räucherlachs-Meerrettich-
+Quark d,g,m,p,2,13  Salatbeilage c,g,k,p Schokopudding g,p</t>
+  </si>
+  <si>
+    <t>Gemüseeintopf m. Kartoffel i Rauchfleisch (50g) 1,2  Baguette a,a-1 Quarkspeise m. Pfirsich g,p</t>
+  </si>
+  <si>
+    <t>Gnocchi-Gemüse-Pfanne c,2  Käsesoße g,p,12  Hähnchenbruststreifen (80g)  Birne 14</t>
+  </si>
+  <si>
+    <t>Kichererbsen-Gemüseragout i Rindfleisch  Couscous a,i,a-1 Streuselkuchen a,c,g,p,a-1,2</t>
+  </si>
+  <si>
+    <t>Lasagne Bolognese a,c,g,i,p,a-
+1,2  Fruchtige Tomatensoße a,a-5 Bohnensalat  Banane</t>
+  </si>
+  <si>
+    <t>Matjesfilettopf "Hausfrauen Art" c,d,g,k,p,1,3,4,12  Röstkartoffeln 2  Salatbeilage c,g,k,p Götterspeise 12</t>
+  </si>
+  <si>
+    <t>Chili con Carne (Rind) 1  Baguette a,a-1 Frucht - Joghurt Dessert g,p</t>
+  </si>
+  <si>
+    <t>Lyoner Wurstsalat i,k,1,2,4,16  Röstkartoffeln 2  Apfel 14</t>
+  </si>
+  <si>
+    <t>Putenkeule geschmort a,c,f,g,i,k,p,2  Champignon-Gemüsesoße g,p Spätzle a,c,a-1 Pfirsichkuchen a,c,a-1,2</t>
+  </si>
+  <si>
+    <t>Bauernfrühstück c,g,p,1,2,16  Gewürzgurke 1,4  Salatbeilage c,g,k,p Honigmelone</t>
+  </si>
+  <si>
+    <t>Fischstäbchen a,d,a-1 Mayonaise-Kartoffelsalat c,k,12  Vanillepudding g,p,12</t>
+  </si>
+  <si>
+    <t>Nudel-Gemüseauflauf a,g,p,a-
+1,2  Tomaten-Kräuterpestosoße 2  Joghurt m. Kirsche g,p,2</t>
+  </si>
+  <si>
+    <t>Asia-Geschnetzeltes mit To-
+fu f,i,m,2,6,13  Reis  Banane</t>
+  </si>
+  <si>
+    <t>Falafelbällchen a,a-1 Joghurt-Minz-Dip g,p Gemüse Couscous a,i,a-1 Apfelkuchen a,c,a-1,2,14</t>
+  </si>
+  <si>
+    <t>Milchreis g,p heiße Kirschen  Birne 14</t>
+  </si>
+  <si>
+    <t>Zucchini Piccata a,c,g,p,a-1 Tomaten-Basilikumsauce g,p,2  Farfalle (Pasta/Nudeln) a,a-1,2  Pudding Sahne c,g,p</t>
+  </si>
+  <si>
+    <t>Penne a,a-1,2  geriebener Käse g,p Gemüse-Sahnesoße g,p Froop g,p</t>
+  </si>
+  <si>
+    <t>gebackener Hirtenkäse g,p Tzatziki g,p Reis  Tomaten-Gurkensalat  Apfel 14</t>
+  </si>
+  <si>
+    <t>Gemüse-Quiche a,c,g,p,a-1 Kräuter-Dip g,p Salatbeilage c,g,k,p Zitronenkuchen a,c,a-1,2</t>
+  </si>
+  <si>
+    <t>gebackene Frühlingsrolle a,c,f,a-1 Ananassauce 8  Gemüsereis  Pfirsich</t>
+  </si>
+  <si>
+    <t>Käsespätzle a,c,g,p,a-1 Geschmolzene Zwiebeln 2  Salatbeilage c,g,k,p Schokopudding g,p</t>
+  </si>
+  <si>
+    <t>Gemüseeintopf m. Kartoffel i Baguette a,a-1 Quarkspeise m. Pfirsich g,p</t>
+  </si>
+  <si>
+    <t>Gnocchi-Gemüse-Pfanne c,2  Käsesoße g,p,12  Birne 14</t>
+  </si>
+  <si>
+    <t>Kichererbsen-Gemüseragout i Couscous a,i,a-1 Streuselkuchen a,c,g,p,a-1,2</t>
+  </si>
+  <si>
+    <t>Gemüselasagne a,c,g,p,a-1,2  Fruchtige Tomatensoße a,a-5 Bohnensalat  Banane</t>
+  </si>
+  <si>
+    <t>Dampfnudel a,c,g,p,a-1 Vanillesoße g,p,12  Götterspeise 12</t>
+  </si>
+  <si>
+    <t>Chili sin Carne (Vegetarisch) a,f,a-1,a-5,1  Baguette a,a-1 Frucht - Joghurt Dessert g,p</t>
+  </si>
+  <si>
+    <t>Gemüsefrikadelle a,b,c,e,f,g,h,i,k,l,m,p,a-1 Schnittlauchquark g,p Röstkartoffeln 2  Apfel 14</t>
+  </si>
+  <si>
+    <t>Spätzle a,c,a-1 Champignon-Gemüseragout g,p Pfirsichkuchen a,c,a-1,2</t>
+  </si>
+  <si>
+    <t>Bauernfrühstück VEG c,g,p Gewürzgurke 1,4  Salatbeilage c,g,k,p Honigmelone</t>
+  </si>
+  <si>
+    <t>Gemüsestäbchen gebraten a,c,g,i,p,a-1 Mayonaise-Kartoffelsalat c,k,12  Vanillepudding g,p,12</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Entferne Nachtisch von menü
</commit_message>
<xml_diff>
--- a/new_merged_menu.xlsx
+++ b/new_merged_menu.xlsx
@@ -25,190 +25,184 @@
     <t>Vegetarisch</t>
   </si>
   <si>
-    <t>2023-06-12</t>
-  </si>
-  <si>
-    <t>2023-06-13</t>
-  </si>
-  <si>
-    <t>2023-06-14</t>
-  </si>
-  <si>
-    <t>2023-06-15</t>
-  </si>
-  <si>
-    <t>2023-06-16</t>
-  </si>
-  <si>
-    <t>2023-06-05</t>
-  </si>
-  <si>
-    <t>2023-06-06</t>
-  </si>
-  <si>
-    <t>2023-06-07</t>
-  </si>
-  <si>
-    <t>2023-06-08</t>
-  </si>
-  <si>
-    <t>2023-06-09</t>
-  </si>
-  <si>
-    <t>2023-06-19</t>
-  </si>
-  <si>
-    <t>2023-06-20</t>
-  </si>
-  <si>
-    <t>2023-06-21</t>
-  </si>
-  <si>
-    <t>2023-06-22</t>
-  </si>
-  <si>
-    <t>2023-06-23</t>
-  </si>
-  <si>
-    <t>2023-06-26</t>
-  </si>
-  <si>
-    <t>2023-06-27</t>
-  </si>
-  <si>
-    <t>2023-06-28</t>
-  </si>
-  <si>
-    <t>2023-06-29</t>
-  </si>
-  <si>
-    <t>2023-06-30</t>
-  </si>
-  <si>
-    <t>Penne a,a-1,2  ger. Putenbrust 1,2,16  Gemüse-Sahnesoße g,p Froop g,p</t>
-  </si>
-  <si>
-    <t>Putengyros 2  Tzatziki g,p Reis  Tomaten-Gurkensalat  Apfel 14</t>
-  </si>
-  <si>
-    <t>Gemüse-Quiche mit Räu-
-chelachs a,c,d,g,p,a-1 Salatbeilage c,g,k,p Zitronenkuchen a,c,a-1,2</t>
-  </si>
-  <si>
-    <t>Chicken Nuggets a,a-1,16  Ananassauce 8  Gemüsereis  Pfirsich</t>
-  </si>
-  <si>
-    <t>Mini Ofenkartoffeln 2  Räucherlachs-Meerrettich-
-Quark d,g,m,p,2,13  Salatbeilage c,g,k,p Schokopudding g,p</t>
-  </si>
-  <si>
-    <t>Nudel-Gemüseauflauf m. Fleisch a,g,p,a-1,2  Tomaten-Kräuterpestosoße 2  Joghurt m. Kirsche g,p,2</t>
-  </si>
-  <si>
-    <t>Asia-Geschnetzeltes vom Huhn i,m,2,6,13  Reis  Banane</t>
-  </si>
-  <si>
-    <t>Hackfleischmasse - Frikadel-
-le/Hackbraten (Rind) a,c,k,a-1 Joghurt-Minz-Dip g,p Gemüse Couscous a,i,a-1 Apfelkuchen a,c,a-1,2,14</t>
-  </si>
-  <si>
-    <t>Hähnchenbrust paniert a,a-1 Bratensoße  Kartoffelpüree g,m,p,2  Sommergemüse  Birne 14</t>
-  </si>
-  <si>
-    <t>Fischfilet Piccata a,c,d,g,p,a-1 Farfalle (Pasta/Nudeln) a,a-1,2  Tomatisierte Zucchini  Pudding Sahne c,g,p</t>
-  </si>
-  <si>
-    <t>Gemüseeintopf m. Kartoffel i Rauchfleisch (50g) 1,2  Baguette a,a-1 Quarkspeise m. Pfirsich g,p</t>
-  </si>
-  <si>
-    <t>Gnocchi-Gemüse-Pfanne c,2  Käsesoße g,p,12  Hähnchenbruststreifen (80g)  Birne 14</t>
-  </si>
-  <si>
-    <t>Kichererbsen-Gemüseragout i Rindfleisch  Couscous a,i,a-1 Streuselkuchen a,c,g,p,a-1,2</t>
-  </si>
-  <si>
-    <t>Lasagne Bolognese a,c,g,i,p,a-
-1,2  Fruchtige Tomatensoße a,a-5 Bohnensalat  Banane</t>
-  </si>
-  <si>
-    <t>Matjesfilettopf "Hausfrauen Art" c,d,g,k,p,1,3,4,12  Röstkartoffeln 2  Salatbeilage c,g,k,p Götterspeise 12</t>
-  </si>
-  <si>
-    <t>Chili con Carne (Rind) 1  Baguette a,a-1 Frucht - Joghurt Dessert g,p</t>
-  </si>
-  <si>
-    <t>Lyoner Wurstsalat i,k,1,2,4,16  Röstkartoffeln 2  Apfel 14</t>
-  </si>
-  <si>
-    <t>Putenkeule geschmort a,c,f,g,i,k,p,2  Champignon-Gemüsesoße g,p Spätzle a,c,a-1 Pfirsichkuchen a,c,a-1,2</t>
-  </si>
-  <si>
-    <t>Bauernfrühstück c,g,p,1,2,16  Gewürzgurke 1,4  Salatbeilage c,g,k,p Honigmelone</t>
-  </si>
-  <si>
-    <t>Fischstäbchen a,d,a-1 Mayonaise-Kartoffelsalat c,k,12  Vanillepudding g,p,12</t>
-  </si>
-  <si>
-    <t>Penne a,a-1,2  geriebener Käse g,p Gemüse-Sahnesoße g,p Froop g,p</t>
-  </si>
-  <si>
-    <t>gebackener Hirtenkäse g,p Tzatziki g,p Reis  Tomaten-Gurkensalat  Apfel 14</t>
-  </si>
-  <si>
-    <t>Gemüse-Quiche a,c,g,p,a-1 Kräuter-Dip g,p Salatbeilage c,g,k,p Zitronenkuchen a,c,a-1,2</t>
-  </si>
-  <si>
-    <t>gebackene Frühlingsrolle a,c,f,a-1 Ananassauce 8  Gemüsereis  Pfirsich</t>
-  </si>
-  <si>
-    <t>Käsespätzle a,c,g,p,a-1 Geschmolzene Zwiebeln 2  Salatbeilage c,g,k,p Schokopudding g,p</t>
-  </si>
-  <si>
-    <t>Nudel-Gemüseauflauf a,g,p,a-
-1,2  Tomaten-Kräuterpestosoße 2  Joghurt m. Kirsche g,p,2</t>
-  </si>
-  <si>
-    <t>Asia-Geschnetzeltes mit To-
-fu f,i,m,2,6,13  Reis  Banane</t>
-  </si>
-  <si>
-    <t>Falafelbällchen a,a-1 Joghurt-Minz-Dip g,p Gemüse Couscous a,i,a-1 Apfelkuchen a,c,a-1,2,14</t>
-  </si>
-  <si>
-    <t>Milchreis g,p heiße Kirschen  Birne 14</t>
-  </si>
-  <si>
-    <t>Zucchini Piccata a,c,g,p,a-1 Tomaten-Basilikumsauce g,p,2  Farfalle (Pasta/Nudeln) a,a-1,2  Pudding Sahne c,g,p</t>
-  </si>
-  <si>
-    <t>Gemüseeintopf m. Kartoffel i Baguette a,a-1 Quarkspeise m. Pfirsich g,p</t>
-  </si>
-  <si>
-    <t>Gnocchi-Gemüse-Pfanne c,2  Käsesoße g,p,12  Birne 14</t>
-  </si>
-  <si>
-    <t>Kichererbsen-Gemüseragout i Couscous a,i,a-1 Streuselkuchen a,c,g,p,a-1,2</t>
-  </si>
-  <si>
-    <t>Gemüselasagne a,c,g,p,a-1,2  Fruchtige Tomatensoße a,a-5 Bohnensalat  Banane</t>
-  </si>
-  <si>
-    <t>Dampfnudel a,c,g,p,a-1 Vanillesoße g,p,12  Götterspeise 12</t>
-  </si>
-  <si>
-    <t>Chili sin Carne (Vegetarisch) a,f,a-1,a-5,1  Baguette a,a-1 Frucht - Joghurt Dessert g,p</t>
-  </si>
-  <si>
-    <t>Gemüsefrikadelle a,b,c,e,f,g,h,i,k,l,m,p,a-1 Schnittlauchquark g,p Röstkartoffeln 2  Apfel 14</t>
-  </si>
-  <si>
-    <t>Spätzle a,c,a-1 Champignon-Gemüseragout g,p Pfirsichkuchen a,c,a-1,2</t>
-  </si>
-  <si>
-    <t>Bauernfrühstück VEG c,g,p Gewürzgurke 1,4  Salatbeilage c,g,k,p Honigmelone</t>
-  </si>
-  <si>
-    <t>Gemüsestäbchen gebraten a,c,g,i,p,a-1 Mayonaise-Kartoffelsalat c,k,12  Vanillepudding g,p,12</t>
+    <t>2024-03-04</t>
+  </si>
+  <si>
+    <t>2024-03-05</t>
+  </si>
+  <si>
+    <t>2024-03-06</t>
+  </si>
+  <si>
+    <t>2024-03-07</t>
+  </si>
+  <si>
+    <t>2024-03-08</t>
+  </si>
+  <si>
+    <t>2024-03-25</t>
+  </si>
+  <si>
+    <t>2024-03-26</t>
+  </si>
+  <si>
+    <t>2024-03-27</t>
+  </si>
+  <si>
+    <t>2024-03-28</t>
+  </si>
+  <si>
+    <t>2024-03-29</t>
+  </si>
+  <si>
+    <t>2024-03-11</t>
+  </si>
+  <si>
+    <t>2024-03-12</t>
+  </si>
+  <si>
+    <t>2024-03-13</t>
+  </si>
+  <si>
+    <t>2024-03-14</t>
+  </si>
+  <si>
+    <t>2024-03-15</t>
+  </si>
+  <si>
+    <t>2024-03-18</t>
+  </si>
+  <si>
+    <t>2024-03-19</t>
+  </si>
+  <si>
+    <t>2024-03-20</t>
+  </si>
+  <si>
+    <t>2024-03-21</t>
+  </si>
+  <si>
+    <t>2024-03-22</t>
+  </si>
+  <si>
+    <t>Erbseneintopf i Baguette a,a-1 Wiener Würstchen 1,2,16</t>
+  </si>
+  <si>
+    <t>Currywurst  Currywurstsoße 1  Mayonaise-Kartoffelsalat c,k,12</t>
+  </si>
+  <si>
+    <t>Frikadelle a,c,a-1 Kartoffeln  Champignon-Gemüseragout g,p</t>
+  </si>
+  <si>
+    <t>Hühnerfrikassee g,p Reis</t>
+  </si>
+  <si>
+    <t>Fischfilet d Kräutersoße g,p Kartoffeln  Blattspinat</t>
+  </si>
+  <si>
+    <t>Chili con Carne (Rind) 1  Baguette a,a-1</t>
+  </si>
+  <si>
+    <t>Fleischkäse 1,2,16  Süßer Senf k Röstkartoffeln 2  Bayrisch Kraut</t>
+  </si>
+  <si>
+    <t>Putenkeule geschmort a,c,f,g,i,k,p,2  Champignon-Gemüsesoße g,p Kräuterspätzle a,c,a-1</t>
+  </si>
+  <si>
+    <t>Bauernfrühstück c,g,p,1,2,16  Gewürzgurke 1,4  Salatbeilage c,g,k,p</t>
+  </si>
+  <si>
+    <t>Fischstäbchen a,d,a-1 Kartoffeln  Rahmspinat g,p</t>
+  </si>
+  <si>
+    <t>Karotten-Weißkohleintopf g,p Baguette a,a-1 Kassler Einlage 1,2</t>
+  </si>
+  <si>
+    <t>Penne a,a-1,2  Arrabiatasoße mit Speck 1,2  Salatbeilage c,g,k,p</t>
+  </si>
+  <si>
+    <t>Hähnchenstreifen Zürcher Art g,p Spätzle a,c,a-1</t>
+  </si>
+  <si>
+    <t>Kohlwurst k,1,2,3,16  Senf k Röstkartoffeln 2  Grünkohl k,1,2,3,16</t>
+  </si>
+  <si>
+    <t>Fischfilet d Finkenwerder Garnitur 1,2  Kartoffeln  Gurkensalat in Dill-Sahne- Joghurt-Dressing g,p</t>
+  </si>
+  <si>
+    <t>Tomatisierter Gemüseeintopf  Baguette a,a-1 Chorizo f,g,p,1,2,12,16</t>
+  </si>
+  <si>
+    <t>Kohlroulade g,k,p Kümmel-Specksoße 1,2  Kartoffeln</t>
+  </si>
+  <si>
+    <t>Hähnchenschnitte gefüllt a,g,i,p,a-1 Kartoffelpüree g,m,p,2  gestovter Rosenkohl g,p</t>
+  </si>
+  <si>
+    <t>Schweinebraten 2  Bratensoße  Röstkartoffeln 2  Kohlrabi g,p</t>
+  </si>
+  <si>
+    <t>Überbackenes Schlemmerfi- let a,c,d,g,p,a-1 Kartoffeln  Wurzelgemüse gestovt g,i,p</t>
+  </si>
+  <si>
+    <t>Erbseneintopf i Baguette a,a-1</t>
+  </si>
+  <si>
+    <t>Tofuwurst (Curry Brat) a,c,a-1 Currywurstsoße 1  Mayonaise-Kartoffelsalat c,k,12</t>
+  </si>
+  <si>
+    <t>Champignonpfanne g,p Semmelknödel a,c,a-1</t>
+  </si>
+  <si>
+    <t>Bohnen-Gemüseeintopf to- matisiert  Baguette a,a-1</t>
+  </si>
+  <si>
+    <t>Vegetarische Maultaschen a,c,g,i,p,a-1 Kräutersoße g,p Blattspinat</t>
+  </si>
+  <si>
+    <t>Chili sin Carne (Vegetarisch) a,f,a-1,a-5,1  Baguette a,a-1</t>
+  </si>
+  <si>
+    <t>Gemüsefrikadelle a,b,c,e,f,g,h,i,k,l,m,p,a-1 Röstkartoffeln 2  Bayrisch Kraut</t>
+  </si>
+  <si>
+    <t>Kräuterspätzle a,c,a-1 Champignon-Gemüseragout g,p</t>
+  </si>
+  <si>
+    <t>Bauernfrühstück VEG c,g,p Gewürzgurke 1,4  Salatbeilage c,g,k,p</t>
+  </si>
+  <si>
+    <t>Gemüsestäbchen gebraten a,c,g,i,p,a-1 Kartoffeln  Rahmspinat g,p</t>
+  </si>
+  <si>
+    <t>Karotten-Weißkohleintopf g,p Baguette a,a-1</t>
+  </si>
+  <si>
+    <t>Penne a,a-1,2  Arrabiatasoße mit Mozzarel- la g,p,1  Salatbeilage c,g,k,p</t>
+  </si>
+  <si>
+    <t>Tofugeschnetzeltes Zürcher Art f,g,p Spätzle a,c,a-1</t>
+  </si>
+  <si>
+    <t>Spanische Gemüsepfanne  Hirtenkäse (30g) g,p Röstkartoffeln 2  Sour Cream g,p,2</t>
+  </si>
+  <si>
+    <t>Paprika-Kartoffelcurry g,i,p,1  Koriander-Dip g,p</t>
+  </si>
+  <si>
+    <t>Tomatisierter Gemüseeintopf  Baguette a,a-1</t>
+  </si>
+  <si>
+    <t>Kohlroulade VEG a,c,f,a-1,a-2 Kümmel-Kräutersoße  Kartoffeln</t>
+  </si>
+  <si>
+    <t>Brokkoli-Kartoffelauflauf g,p</t>
+  </si>
+  <si>
+    <t>Roter Linsenbratling a,b,c,e,f,g,h,i,k,l,m,p Bratensoße  Röstkartoffeln 2  Kohlrabi g,p</t>
+  </si>
+  <si>
+    <t>Eieromelette c,g,p Kartoffeln  Wurzelgemüse gestovt g,i,p</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
add Windows to Readme improved special char filtering
</commit_message>
<xml_diff>
--- a/new_merged_menu.xlsx
+++ b/new_merged_menu.xlsx
@@ -25,184 +25,252 @@
     <t>Vegetarisch</t>
   </si>
   <si>
-    <t>2024-03-04</t>
-  </si>
-  <si>
-    <t>2024-03-05</t>
-  </si>
-  <si>
-    <t>2024-03-06</t>
-  </si>
-  <si>
-    <t>2024-03-07</t>
-  </si>
-  <si>
-    <t>2024-03-08</t>
-  </si>
-  <si>
-    <t>2024-03-25</t>
-  </si>
-  <si>
-    <t>2024-03-26</t>
-  </si>
-  <si>
-    <t>2024-03-27</t>
-  </si>
-  <si>
-    <t>2024-03-28</t>
-  </si>
-  <si>
-    <t>2024-03-29</t>
-  </si>
-  <si>
-    <t>2024-03-11</t>
-  </si>
-  <si>
-    <t>2024-03-12</t>
-  </si>
-  <si>
-    <t>2024-03-13</t>
-  </si>
-  <si>
-    <t>2024-03-14</t>
-  </si>
-  <si>
-    <t>2024-03-15</t>
-  </si>
-  <si>
-    <t>2024-03-18</t>
-  </si>
-  <si>
-    <t>2024-03-19</t>
-  </si>
-  <si>
-    <t>2024-03-20</t>
-  </si>
-  <si>
-    <t>2024-03-21</t>
-  </si>
-  <si>
-    <t>2024-03-22</t>
-  </si>
-  <si>
-    <t>Erbseneintopf i Baguette a,a-1 Wiener Würstchen 1,2,16</t>
-  </si>
-  <si>
-    <t>Currywurst  Currywurstsoße 1  Mayonaise-Kartoffelsalat c,k,12</t>
-  </si>
-  <si>
-    <t>Frikadelle a,c,a-1 Kartoffeln  Champignon-Gemüseragout g,p</t>
-  </si>
-  <si>
-    <t>Hühnerfrikassee g,p Reis</t>
-  </si>
-  <si>
-    <t>Fischfilet d Kräutersoße g,p Kartoffeln  Blattspinat</t>
-  </si>
-  <si>
-    <t>Chili con Carne (Rind) 1  Baguette a,a-1</t>
-  </si>
-  <si>
-    <t>Fleischkäse 1,2,16  Süßer Senf k Röstkartoffeln 2  Bayrisch Kraut</t>
-  </si>
-  <si>
-    <t>Putenkeule geschmort a,c,f,g,i,k,p,2  Champignon-Gemüsesoße g,p Kräuterspätzle a,c,a-1</t>
-  </si>
-  <si>
-    <t>Bauernfrühstück c,g,p,1,2,16  Gewürzgurke 1,4  Salatbeilage c,g,k,p</t>
-  </si>
-  <si>
-    <t>Fischstäbchen a,d,a-1 Kartoffeln  Rahmspinat g,p</t>
-  </si>
-  <si>
-    <t>Karotten-Weißkohleintopf g,p Baguette a,a-1 Kassler Einlage 1,2</t>
-  </si>
-  <si>
-    <t>Penne a,a-1,2  Arrabiatasoße mit Speck 1,2  Salatbeilage c,g,k,p</t>
-  </si>
-  <si>
-    <t>Hähnchenstreifen Zürcher Art g,p Spätzle a,c,a-1</t>
-  </si>
-  <si>
-    <t>Kohlwurst k,1,2,3,16  Senf k Röstkartoffeln 2  Grünkohl k,1,2,3,16</t>
-  </si>
-  <si>
-    <t>Fischfilet d Finkenwerder Garnitur 1,2  Kartoffeln  Gurkensalat in Dill-Sahne- Joghurt-Dressing g,p</t>
-  </si>
-  <si>
-    <t>Tomatisierter Gemüseeintopf  Baguette a,a-1 Chorizo f,g,p,1,2,12,16</t>
-  </si>
-  <si>
-    <t>Kohlroulade g,k,p Kümmel-Specksoße 1,2  Kartoffeln</t>
-  </si>
-  <si>
-    <t>Hähnchenschnitte gefüllt a,g,i,p,a-1 Kartoffelpüree g,m,p,2  gestovter Rosenkohl g,p</t>
-  </si>
-  <si>
-    <t>Schweinebraten 2  Bratensoße  Röstkartoffeln 2  Kohlrabi g,p</t>
-  </si>
-  <si>
-    <t>Überbackenes Schlemmerfi- let a,c,d,g,p,a-1 Kartoffeln  Wurzelgemüse gestovt g,i,p</t>
-  </si>
-  <si>
-    <t>Erbseneintopf i Baguette a,a-1</t>
-  </si>
-  <si>
-    <t>Tofuwurst (Curry Brat) a,c,a-1 Currywurstsoße 1  Mayonaise-Kartoffelsalat c,k,12</t>
-  </si>
-  <si>
-    <t>Champignonpfanne g,p Semmelknödel a,c,a-1</t>
-  </si>
-  <si>
-    <t>Bohnen-Gemüseeintopf to- matisiert  Baguette a,a-1</t>
-  </si>
-  <si>
-    <t>Vegetarische Maultaschen a,c,g,i,p,a-1 Kräutersoße g,p Blattspinat</t>
-  </si>
-  <si>
-    <t>Chili sin Carne (Vegetarisch) a,f,a-1,a-5,1  Baguette a,a-1</t>
-  </si>
-  <si>
-    <t>Gemüsefrikadelle a,b,c,e,f,g,h,i,k,l,m,p,a-1 Röstkartoffeln 2  Bayrisch Kraut</t>
-  </si>
-  <si>
-    <t>Kräuterspätzle a,c,a-1 Champignon-Gemüseragout g,p</t>
-  </si>
-  <si>
-    <t>Bauernfrühstück VEG c,g,p Gewürzgurke 1,4  Salatbeilage c,g,k,p</t>
-  </si>
-  <si>
-    <t>Gemüsestäbchen gebraten a,c,g,i,p,a-1 Kartoffeln  Rahmspinat g,p</t>
-  </si>
-  <si>
-    <t>Karotten-Weißkohleintopf g,p Baguette a,a-1</t>
-  </si>
-  <si>
-    <t>Penne a,a-1,2  Arrabiatasoße mit Mozzarel- la g,p,1  Salatbeilage c,g,k,p</t>
-  </si>
-  <si>
-    <t>Tofugeschnetzeltes Zürcher Art f,g,p Spätzle a,c,a-1</t>
-  </si>
-  <si>
-    <t>Spanische Gemüsepfanne  Hirtenkäse (30g) g,p Röstkartoffeln 2  Sour Cream g,p,2</t>
-  </si>
-  <si>
-    <t>Paprika-Kartoffelcurry g,i,p,1  Koriander-Dip g,p</t>
-  </si>
-  <si>
-    <t>Tomatisierter Gemüseeintopf  Baguette a,a-1</t>
-  </si>
-  <si>
-    <t>Kohlroulade VEG a,c,f,a-1,a-2 Kümmel-Kräutersoße  Kartoffeln</t>
-  </si>
-  <si>
-    <t>Brokkoli-Kartoffelauflauf g,p</t>
-  </si>
-  <si>
-    <t>Roter Linsenbratling a,b,c,e,f,g,h,i,k,l,m,p Bratensoße  Röstkartoffeln 2  Kohlrabi g,p</t>
-  </si>
-  <si>
-    <t>Eieromelette c,g,p Kartoffeln  Wurzelgemüse gestovt g,i,p</t>
+    <t>2024-05-06</t>
+  </si>
+  <si>
+    <t>2024-05-07</t>
+  </si>
+  <si>
+    <t>2024-05-08</t>
+  </si>
+  <si>
+    <t>2024-05-09</t>
+  </si>
+  <si>
+    <t>2024-05-10</t>
+  </si>
+  <si>
+    <t>2024-05-13</t>
+  </si>
+  <si>
+    <t>2024-05-14</t>
+  </si>
+  <si>
+    <t>2024-05-15</t>
+  </si>
+  <si>
+    <t>2024-05-16</t>
+  </si>
+  <si>
+    <t>2024-05-17</t>
+  </si>
+  <si>
+    <t>2024-05-27</t>
+  </si>
+  <si>
+    <t>2024-05-28</t>
+  </si>
+  <si>
+    <t>2024-05-29</t>
+  </si>
+  <si>
+    <t>2024-05-30</t>
+  </si>
+  <si>
+    <t>2024-05-31</t>
+  </si>
+  <si>
+    <t>2024-05-20</t>
+  </si>
+  <si>
+    <t>2024-05-21</t>
+  </si>
+  <si>
+    <t>2024-05-22</t>
+  </si>
+  <si>
+    <t>2024-05-23</t>
+  </si>
+  <si>
+    <t>2024-05-24</t>
+  </si>
+  <si>
+    <t>Hähnchenstreifen "Zürcher Art" g,p
+Butternudeln a,g,p,a-1,2</t>
+  </si>
+  <si>
+    <t>Kasslerbraten kalt 1,2 
+Remoulade c,g,k,p,1,4,12 
+Röstkartoffeln 2 
+Salatbeilage c,g,k,p</t>
+  </si>
+  <si>
+    <t>Tortellini (Fleisch) a,c,g,p,a-1,1,2 
+Gemüse-Sahnesoße g,p</t>
+  </si>
+  <si>
+    <t>Hühnerfrikassee g,p
+Reis</t>
+  </si>
+  <si>
+    <t>Ofenkartoffel 
+Dill-Heringshappen-Ragout d,g,p,1 
+Salatbeilage c,g,k,p</t>
+  </si>
+  <si>
+    <t>Nudel-Gemüseauflauf m. Fleisch a,g,p,a-1,2 
+Tomaten-Kräuterpestosoße 2</t>
+  </si>
+  <si>
+    <t>Asia-Geschnetzeltes vom Huhn i,m,2,6,13 
+Reis</t>
+  </si>
+  <si>
+    <t>Hackfleischmasse - Frikadelle/Hackbraten (Rind) a,c,k,a-1
+Joghurt-Minz-Dip g,p
+Gemüse Couscous a,i,a-1</t>
+  </si>
+  <si>
+    <t>Hähnchenbrust paniert a,a-1
+Bratensoße 
+Kartoffelpüree g,m,p,2 
+Sommergemüse</t>
+  </si>
+  <si>
+    <t>Fischfilet Piccata a,c,d,g,p,a-1
+Farfalle (Pasta/Nudeln) a,a-1,2 
+Tomatisierte Zucchini</t>
+  </si>
+  <si>
+    <t>Gemüseeintopf m. Kartoffel i
+Rauchfleisch (50g) 1,2 
+Baguette a,a-1</t>
+  </si>
+  <si>
+    <t>Gnocchi-Gemüse-Pfanne c,2 
+Käsesoße g,p,12 
+Hähnchenbruststreifen (80g)</t>
+  </si>
+  <si>
+    <t>Kichererbsen-Gemüseragout i
+Rindfleisch 
+Couscous a,i,a-1</t>
+  </si>
+  <si>
+    <t>Lasagne Bolognese a,c,g,i,p,a1,2 
+Fruchtige Tomatensoße a,a-5
+Bohnensalat</t>
+  </si>
+  <si>
+    <t>Matjesfilettopf "HausfrauenArt" c,d,g,k,p,1,3,4,12 
+Röstkartoffeln 2 
+Salatbeilage c,g,k,p</t>
+  </si>
+  <si>
+    <t>Penne a,a-1,2 
+ger. Putenbrust 1,2,16 
+Gemüse-Sahnesoße g,p</t>
+  </si>
+  <si>
+    <t>Putengyros 2 
+Tzatziki g,p
+Reis 
+Tomaten-Gurkensalat</t>
+  </si>
+  <si>
+    <t>Gemüse-Quiche mit Räuchelachs a,c,d,g,p,a-1
+Salatbeilage c,g,k,p</t>
+  </si>
+  <si>
+    <t>Chicken Nuggets a,a-1,16 
+Ananassauce 8 
+Gemüsereis</t>
+  </si>
+  <si>
+    <t>Mini Ofenkartoffeln 2 
+Räucherlachs-MeerrettichQuark d,g,m,p,2,13 
+Salatbeilage c,g,k,p</t>
+  </si>
+  <si>
+    <t>Tofugeschnetzeltes "Zürcher Art" f,g,p
+Butternudeln a,g,p,a-1,2</t>
+  </si>
+  <si>
+    <t>Makkaroni a,c,a-1,2 
+Zucchini-Paprika in Pestosoße g,p,2</t>
+  </si>
+  <si>
+    <t>Tortellini (Vegetarisch) a,c,g,p,a-1,2 
+Gemüse-Sahnesoße g,p</t>
+  </si>
+  <si>
+    <t>Vegetarische Maultaschen a,c,g,i,p,a-1
+Geschmorte Butterzwiebeln g,p
+Rohkost / Gemüsesticks</t>
+  </si>
+  <si>
+    <t>Ofenkartoffel 
+Rucola-Dörrtomatencreme g,m,p,2 
+Salatbeilage c,g,k,p</t>
+  </si>
+  <si>
+    <t>Nudel-Gemüseauflauf a,g,p,a1,2 
+Tomaten-Kräuterpestosoße 2</t>
+  </si>
+  <si>
+    <t>Asia-Geschnetzeltes mit Tofu f,i,m,2,6,13 
+Reis</t>
+  </si>
+  <si>
+    <t>Falafelbällchen a,a-1
+Joghurt-Minz-Dip g,p
+Gemüse Couscous a,i,a-1</t>
+  </si>
+  <si>
+    <t>Milchreis g,p
+heiße Kirschen</t>
+  </si>
+  <si>
+    <t>Zucchini Piccata a,c,g,p,a-1
+Tomaten-Basilikumsauce g,p,2 
+Farfalle (Pasta/Nudeln) a,a-1,2</t>
+  </si>
+  <si>
+    <t>Gemüseeintopf m. Kartoffel i
+Baguette a,a-1</t>
+  </si>
+  <si>
+    <t>Gnocchi-Gemüse-Pfanne c,2 
+Käsesoße g,p,12</t>
+  </si>
+  <si>
+    <t>Kichererbsen-Gemüseragout i
+Couscous a,i,a-1</t>
+  </si>
+  <si>
+    <t>Gemüselasagne a,c,g,p,a-1,2 
+Fruchtige Tomatensoße a,a-5
+Bohnensalat</t>
+  </si>
+  <si>
+    <t>Dampfnudel a,c,g,p,a-1
+Vanillesoße g,p,12</t>
+  </si>
+  <si>
+    <t>Penne a,a-1,2 
+geriebener Käse g,p
+Gemüse-Sahnesoße g,p</t>
+  </si>
+  <si>
+    <t>gebackener Hirtenkäse g,p
+Tzatziki g,p
+Reis 
+Tomaten-Gurkensalat</t>
+  </si>
+  <si>
+    <t>Gemüse-Quiche a,c,g,p,a-1
+Kräuter-Dip g,p
+Salatbeilage c,g,k,p</t>
+  </si>
+  <si>
+    <t>gebackene Frühlingsrolle a,c,f,a-1
+Ananassauce 8 
+Gemüsereis</t>
+  </si>
+  <si>
+    <t>Käsespätzle a,c,g,p,a-1
+Geschmolzene Zwiebeln 2 
+Salatbeilage c,g,k,p</t>
   </si>
 </sst>
 </file>

</xml_diff>